<commit_message>
fix: issue 37, innovation project status
</commit_message>
<xml_diff>
--- a/dattbi.xlsx
+++ b/dattbi.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Project Descriptions" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15562" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15564" uniqueCount="419">
   <si>
     <t>IP</t>
   </si>
@@ -2359,9 +2359,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I55" sqref="I55"/>
+      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6182,16 +6182,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="19"/>
     <col min="2" max="2" width="17.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="3" customWidth="1"/>
     <col min="5" max="5" width="37.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="76.42578125" style="3" customWidth="1"/>
@@ -6399,7 +6399,7 @@
         <v>247</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>364</v>
+        <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -6554,8 +6554,8 @@
       <c r="B13" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="C13" s="3">
-        <v>2</v>
+      <c r="C13" s="3" t="s">
+        <v>297</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>52</v>
@@ -6572,8 +6572,8 @@
       <c r="H13" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="I13" s="3">
-        <v>2</v>
+      <c r="I13" s="3" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -6581,10 +6581,10 @@
         <v>43</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>293</v>
+        <v>43</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>297</v>
+        <v>259</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>80</v>
@@ -6610,10 +6610,10 @@
         <v>45</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>295</v>
+        <v>45</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>297</v>
+        <v>259</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
improve timevis filters and views
</commit_message>
<xml_diff>
--- a/dattbi.xlsx
+++ b/dattbi.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project Descriptions" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15564" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15558" uniqueCount="418">
   <si>
     <t>IP</t>
   </si>
@@ -1470,9 +1470,6 @@
   <si>
     <t>Forecasted Total Expenditures</t>
   </si>
-  <si>
-    <t>3 to 6</t>
-  </si>
 </sst>
 </file>
 
@@ -2359,18 +2356,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="19" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="27" style="10" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" style="10" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" style="10" customWidth="1"/>
     <col min="7" max="7" width="14.140625" style="10" customWidth="1"/>
     <col min="8" max="8" width="23.42578125" style="10" customWidth="1"/>
@@ -2378,7 +2375,7 @@
     <col min="10" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
@@ -2665,8 +2662,8 @@
       <c r="H10" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="I10" s="10" t="s">
-        <v>418</v>
+      <c r="I10" s="10">
+        <v>4.5</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3127,8 +3124,8 @@
       <c r="H26" s="42" t="s">
         <v>361</v>
       </c>
-      <c r="I26" s="10" t="s">
-        <v>418</v>
+      <c r="I26" s="10">
+        <v>4.5</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3154,8 +3151,8 @@
       <c r="H27" s="42" t="s">
         <v>361</v>
       </c>
-      <c r="I27" s="10" t="s">
-        <v>418</v>
+      <c r="I27" s="10">
+        <v>4.5</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3181,8 +3178,8 @@
       <c r="H28" s="42" t="s">
         <v>361</v>
       </c>
-      <c r="I28" s="10" t="s">
-        <v>418</v>
+      <c r="I28" s="10">
+        <v>4.5</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3208,8 +3205,8 @@
       <c r="H29" s="42" t="s">
         <v>361</v>
       </c>
-      <c r="I29" s="10" t="s">
-        <v>418</v>
+      <c r="I29" s="10">
+        <v>4.5</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3235,8 +3232,8 @@
       <c r="H30" s="42" t="s">
         <v>361</v>
       </c>
-      <c r="I30" s="10" t="s">
-        <v>418</v>
+      <c r="I30" s="10">
+        <v>4.5</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3262,8 +3259,8 @@
       <c r="H31" s="42" t="s">
         <v>361</v>
       </c>
-      <c r="I31" s="10" t="s">
-        <v>418</v>
+      <c r="I31" s="10">
+        <v>4.5</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3289,8 +3286,8 @@
       <c r="H32" s="42" t="s">
         <v>361</v>
       </c>
-      <c r="I32" s="10" t="s">
-        <v>418</v>
+      <c r="I32" s="10">
+        <v>4.5</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3374,8 +3371,8 @@
       <c r="H35" s="10" t="s">
         <v>392</v>
       </c>
-      <c r="I35" s="10" t="s">
-        <v>418</v>
+      <c r="I35" s="10">
+        <v>4.5</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -3758,8 +3755,8 @@
       <c r="H49" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="I49" s="10" t="s">
-        <v>418</v>
+      <c r="I49" s="10">
+        <v>4.5</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -3811,13 +3808,13 @@
         <v>44073</v>
       </c>
       <c r="G51" s="15">
-        <v>43880</v>
+        <v>44246</v>
       </c>
       <c r="H51" s="10" t="s">
         <v>254</v>
       </c>
       <c r="I51" s="10">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -4039,7 +4036,7 @@
         <v>260</v>
       </c>
       <c r="I59" s="10">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -4068,7 +4065,7 @@
         <v>260</v>
       </c>
       <c r="I60" s="10">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4096,8 +4093,8 @@
       <c r="H61" s="42" t="s">
         <v>332</v>
       </c>
-      <c r="I61" s="10">
-        <v>6</v>
+      <c r="I61" s="10" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4125,8 +4122,8 @@
       <c r="H62" s="42" t="s">
         <v>332</v>
       </c>
-      <c r="I62" s="10">
-        <v>6</v>
+      <c r="I62" s="10" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4153,7 +4150,7 @@
         <v>332</v>
       </c>
       <c r="I63" s="10">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4180,7 +4177,7 @@
         <v>332</v>
       </c>
       <c r="I64" s="10">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4208,8 +4205,8 @@
       <c r="H65" s="42" t="s">
         <v>332</v>
       </c>
-      <c r="I65" s="10">
-        <v>6</v>
+      <c r="I65" s="10" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4237,11 +4234,11 @@
       <c r="H66" s="42" t="s">
         <v>332</v>
       </c>
-      <c r="I66" s="10">
-        <v>6</v>
+      <c r="I66" s="10" t="s">
+        <v>342</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="48" t="s">
         <v>45</v>
       </c>
@@ -4265,7 +4262,7 @@
         <v>332</v>
       </c>
       <c r="I67" s="10">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4292,7 +4289,7 @@
         <v>332</v>
       </c>
       <c r="I68" s="10">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -6182,7 +6179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>

</xml_diff>